<commit_message>
clean up error file
</commit_message>
<xml_diff>
--- a/ot/utils/static/variant_standardization.xlsx
+++ b/ot/utils/static/variant_standardization.xlsx
@@ -24,56 +24,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
-  <si>
-    <t>No-Limit Hold'em</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>NLH</t>
   </si>
   <si>
-    <t>Limit Hold'em</t>
-  </si>
-  <si>
     <t>LHE</t>
   </si>
   <si>
-    <t>Pot Limit Omaha</t>
-  </si>
-  <si>
     <t>PLO</t>
   </si>
   <si>
-    <t>Pot Limit Omaha High/Low</t>
-  </si>
-  <si>
     <t>PLO-H/LOW</t>
   </si>
   <si>
-    <t>Omaha High/Low</t>
-  </si>
-  <si>
     <t>OMA/HI-LOW</t>
   </si>
   <si>
-    <t>Limit Omaha</t>
-  </si>
-  <si>
     <t>LIMIT OMAHA/HI</t>
   </si>
   <si>
     <t>PLO/8</t>
   </si>
   <si>
-    <t>Pot Limit Omaha 8 or Better</t>
-  </si>
-  <si>
     <t>LO8</t>
   </si>
   <si>
-    <t>Limit Omaha 8 or Better</t>
-  </si>
-  <si>
     <t>NL HOLDEM</t>
   </si>
   <si>
@@ -92,16 +68,46 @@
     <t>LIMIT OMAHA HI</t>
   </si>
   <si>
+    <t>NO-LIMIT HOLD'EM</t>
+  </si>
+  <si>
+    <t>NL HOLD'EM</t>
+  </si>
+  <si>
+    <t>NO LIMIT HOLDEM</t>
+  </si>
+  <si>
+    <t>LIMIT HOLD'EM</t>
+  </si>
+  <si>
+    <t>POT LIMIT OMAHA</t>
+  </si>
+  <si>
+    <t>POT LIMIT OMAHA HIGH/LOW</t>
+  </si>
+  <si>
+    <t>OMAHA HIGH/LOW</t>
+  </si>
+  <si>
+    <t>LIMIT OMAHA</t>
+  </si>
+  <si>
+    <t>POT LIMIT OMAHA 8 OR BETTER</t>
+  </si>
+  <si>
+    <t>LIMIT OMAHA 8 OR BETTER</t>
+  </si>
+  <si>
     <t>NL Holdem</t>
   </si>
   <si>
-    <t>NL Hold'em</t>
-  </si>
-  <si>
     <t>Limit Holdem</t>
   </si>
   <si>
     <t>N/L Holdem</t>
+  </si>
+  <si>
+    <t>No Limit Holdem</t>
   </si>
 </sst>
 </file>
@@ -453,130 +459,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>